<commit_message>
Kvals not needed in mu calculation, hence removed
</commit_message>
<xml_diff>
--- a/tiretrainingdata.xlsx
+++ b/tiretrainingdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarora\Documents\Local\Vehicle Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B345083-BAE1-48EA-8A81-52A1D6B8A4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D7C7A0-877D-477A-8980-D1B84D254BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{10E3E5CB-56F8-4418-A79C-00BCE81C47B9}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{10E3E5CB-56F8-4418-A79C-00BCE81C47B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,7 +419,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C40"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,134 +448,134 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.24025099671004005</v>
+        <v>0.13149684452957783</v>
       </c>
       <c r="B3">
-        <v>0.25247619047619041</v>
+        <v>0.13818807339449543</v>
       </c>
       <c r="C3">
-        <v>0.25247619047619041</v>
+        <v>0.1381880733944954</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.48053859038445579</v>
+        <v>0.26301371971626286</v>
       </c>
       <c r="B4">
-        <v>0.49272108843537404</v>
+        <v>0.2696815798880019</v>
       </c>
       <c r="C4">
-        <v>0.43869166127989645</v>
+        <v>0.24010959359043543</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.72089940028999633</v>
+        <v>0.39457066842394506</v>
       </c>
       <c r="B5">
-        <v>0.71575510204081627</v>
+        <v>0.39175503395686889</v>
       </c>
       <c r="C5">
-        <v>0.56435854341736691</v>
+        <v>0.30889098758769562</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0.96137009032704435</v>
+        <v>0.52618775794589068</v>
       </c>
       <c r="B6">
-        <v>0.91900680272108837</v>
+        <v>0.50300101274871922</v>
       </c>
       <c r="C6">
-        <v>0.61919500107735392</v>
+        <v>0.33890468678650004</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1.2019873914187169</v>
+        <v>0.65788509225899328</v>
       </c>
       <c r="B7">
-        <v>1.0998775510204082</v>
+        <v>0.60199720004765878</v>
       </c>
       <c r="C7">
-        <v>0.61576772247360467</v>
+        <v>0.33702883058657479</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1.4427881239868845</v>
+        <v>0.78968282432559878</v>
       </c>
       <c r="B8">
-        <v>1.2657687074829931</v>
+        <v>0.69279459073037064</v>
       </c>
       <c r="C8">
-        <v>0.56778582202111605</v>
+        <v>0.31076684378762093</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1.6838092205443826</v>
+        <v>0.92160116845892515</v>
       </c>
       <c r="B9">
-        <v>1.4106666666666665</v>
+        <v>0.77210175145954962</v>
       </c>
       <c r="C9">
-        <v>0.46953716871363921</v>
+        <v>0.25699229938976298</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1.9250877484329545</v>
+        <v>1.0536604127682456</v>
       </c>
       <c r="B10">
-        <v>1.5281360544217686</v>
+        <v>0.83639640176337438</v>
       </c>
       <c r="C10">
-        <v>0.32559146735617317</v>
+        <v>0.17820633899290134</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2.1666609327367734</v>
+        <v>1.1858809317001733</v>
       </c>
       <c r="B11">
-        <v>1.6258503401360542</v>
+        <v>0.88987847015369959</v>
       </c>
       <c r="C11">
-        <v>0.15993966817496225</v>
+        <v>8.7539955996512916E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2.408566179401805</v>
+        <v>1.3182831986926062</v>
       </c>
       <c r="B12">
-        <v>1.7062176870748296</v>
+        <v>0.93386601930179902</v>
       </c>
       <c r="C12">
-        <v>-2.0563671622495148E-2</v>
+        <v>-1.1255137199551662E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2.6508410985917212</v>
+        <v>1.4508877989581461</v>
       </c>
       <c r="B13">
-        <v>1.7727482993197277</v>
+        <v>0.97028029310139419</v>
       </c>
       <c r="C13">
-        <v>-0.19421245421245417</v>
+        <v>-0.10629851799576572</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2.8935235283116096</v>
+        <v>1.5837154424140902</v>
       </c>
       <c r="B14">
-        <v>1.8270476190476188</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>-0.3655763843999138</v>
+        <v>-0.20009132799202958</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,134 +591,134 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0.20509704310546614</v>
+        <v>0.12330004493099127</v>
       </c>
       <c r="B16">
-        <v>0.21087755102040812</v>
+        <v>0.12677516517087595</v>
       </c>
       <c r="C16">
-        <v>0.21087755102040812</v>
+        <v>0.12677516517087592</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>0.41022532824231983</v>
+        <v>0.24661887191664064</v>
       </c>
       <c r="B17">
-        <v>0.41596938775510195</v>
+        <v>0.25007208014084764</v>
       </c>
       <c r="C17">
-        <v>0.3792483705524094</v>
+        <v>0.22799617401149677</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0.61541611648099881</v>
+        <v>0.36997527445748429</v>
       </c>
       <c r="B18">
-        <v>0.60816326530612241</v>
+        <v>0.36561501229963256</v>
       </c>
       <c r="C18">
-        <v>0.50897670691313168</v>
+        <v>0.30598613164279481</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0.82070070699470188</v>
+        <v>0.49338806896063986</v>
       </c>
       <c r="B19">
-        <v>0.78648979591836732</v>
+        <v>0.47282118604037709</v>
       </c>
       <c r="C19">
-        <v>0.58129335399081083</v>
+        <v>0.34946138462024179</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1.0261104561724763</v>
+        <v>0.61687610623019451</v>
       </c>
       <c r="B20">
-        <v>0.94689795918367348</v>
+        <v>0.56925521277444135</v>
       </c>
       <c r="C20">
-        <v>0.61331141147558488</v>
+        <v>0.36870996990796634</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1.2316767968065063</v>
+        <v>0.74045828300219996</v>
       </c>
       <c r="B21">
-        <v>1.0962959183673466</v>
+        <v>0.65907013551066462</v>
       </c>
       <c r="C21">
-        <v>0.60116663105032597</v>
+        <v>0.36140878238503643</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1.4374312573785908</v>
+        <v>0.86415355353930001</v>
       </c>
       <c r="B22">
-        <v>1.2314795918367345</v>
+        <v>0.7403397275063951</v>
       </c>
       <c r="C22">
-        <v>0.55755582861416808</v>
+        <v>0.33519088173451489</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1.6434054814710308</v>
+        <v>0.98798094130014802</v>
       </c>
       <c r="B23">
-        <v>1.3499795918367348</v>
+        <v>0.8115794445841743</v>
       </c>
       <c r="C23">
-        <v>0.48689528795811515</v>
+        <v>0.2927112452374675</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>1.8496312473274039</v>
+        <v>1.1119595506989357</v>
       </c>
       <c r="B24">
-        <v>1.4522755102040816</v>
+        <v>0.87307760730739259</v>
       </c>
       <c r="C24">
-        <v>0.40132978950742598</v>
+        <v>0.24127106041682411</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2.0561404875890621</v>
+        <v>1.2361085789705613</v>
       </c>
       <c r="B25">
-        <v>1.5368775510204082</v>
+        <v>0.92393858158551789</v>
       </c>
       <c r="C25">
-        <v>0.29423490757559567</v>
+        <v>0.17688786135098655</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2.2629653092335631</v>
+        <v>1.3604473281571974</v>
       </c>
       <c r="B26">
-        <v>1.6060408163265305</v>
+        <v>0.96551808751449275</v>
       </c>
       <c r="C26">
-        <v>0.17830745806175871</v>
+        <v>0.10719470772301813</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2.4701380137417193</v>
+        <v>1.4849952172322973</v>
       </c>
       <c r="B27">
-        <v>1.6633979591836734</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>6.0723902126295547E-2</v>
+        <v>3.6505937614650139E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -734,134 +734,134 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0.17545751519839933</v>
+        <v>0.12658899588788453</v>
       </c>
       <c r="B29">
-        <v>0.18263673469387753</v>
+        <v>0.13176865539784435</v>
       </c>
       <c r="C29">
-        <v>0.18263673469387753</v>
+        <v>0.13176865539784435</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>0.35094175749687773</v>
+        <v>0.2531972748298929</v>
       </c>
       <c r="B30">
-        <v>0.35808979591836737</v>
+        <v>0.25835443783497258</v>
       </c>
       <c r="C30">
-        <v>0.32293813433419344</v>
+        <v>0.23299323550231871</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>0.5264794702831429</v>
+        <v>0.37984413163133868</v>
       </c>
       <c r="B31">
-        <v>0.52228571428571413</v>
+        <v>0.37681842275752392</v>
       </c>
       <c r="C31">
-        <v>0.42230371412932988</v>
+        <v>0.30468346181072442</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>0.7020974295412562</v>
+        <v>0.50654888461513548</v>
       </c>
       <c r="B32">
-        <v>0.67372244897959177</v>
+        <v>0.48607691854643953</v>
       </c>
       <c r="C32">
-        <v>0.48003371647509574</v>
+        <v>0.34633447357441088</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>0.87782246020259891</v>
+        <v>0.63333088741868404</v>
       </c>
       <c r="B33">
-        <v>0.80955102040816318</v>
+        <v>0.58407444490252658</v>
       </c>
       <c r="C33">
-        <v>0.50382547501759323</v>
+        <v>0.36349973902853616</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>1.0536814525603164</v>
+        <v>0.76020954083655534</v>
       </c>
       <c r="B34">
-        <v>0.93421224489795929</v>
+        <v>0.67401495965604563</v>
       </c>
       <c r="C34">
-        <v>0.50732426303854872</v>
+        <v>0.36602404277178985</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>1.229701378768618</v>
+        <v>0.88720430472439882</v>
       </c>
       <c r="B35">
-        <v>1.0415020408163262</v>
+        <v>0.75142234525001461</v>
       </c>
       <c r="C35">
-        <v>0.48038359527719132</v>
+        <v>0.3465869039487362</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>1.4059093094485051</v>
+        <v>1.0143347099796329</v>
       </c>
       <c r="B36">
-        <v>1.1315673469387755</v>
+        <v>0.81640261499499378</v>
       </c>
       <c r="C36">
-        <v>0.43175044178590977</v>
+        <v>0.31149908191750952</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>1.5823324304217288</v>
+        <v>1.1416203706146522</v>
       </c>
       <c r="B37">
-        <v>1.2096163265306121</v>
+        <v>0.87271335178750198</v>
       </c>
       <c r="C37">
-        <v>0.37681946985690828</v>
+        <v>0.271867513148426</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>1.7589980595950736</v>
+        <v>1.2690809959384917</v>
       </c>
       <c r="B38">
-        <v>1.2777142857142858</v>
+        <v>0.92184463160374552</v>
       </c>
       <c r="C38">
-        <v>0.31734007350066462</v>
+        <v>0.22895434951311272</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>1.9359336640173932</v>
+        <v>1.3967364028631288</v>
       </c>
       <c r="B39">
-        <v>1.3361959183673466</v>
+        <v>0.96403792920666687</v>
       </c>
       <c r="C39">
-        <v>0.26275898037375867</v>
+        <v>0.1895752111183546</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2.113166877132227</v>
+        <v>1.5246065283508909</v>
       </c>
       <c r="B40">
-        <v>1.3860408163265308</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>0.20397934162170611</v>
+        <v>0.14716690823169207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>